<commit_message>
Mise à jour application
</commit_message>
<xml_diff>
--- a/charges.xlsx
+++ b/charges.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fatou Sène Dieng\mon_projet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fatou Sène Dieng\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB50CD3-DD89-403A-8400-CD0EC1D213C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E01E8B-E146-4949-9FDF-141FEA36AA39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="19">
   <si>
     <t>année</t>
   </si>
@@ -419,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33:F34"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="J50" sqref="J50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -465,7 +465,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="2">
-        <v>60000</v>
+        <v>0</v>
       </c>
       <c r="D2" s="2">
         <v>5000</v>
@@ -477,7 +477,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="2">
-        <v>0</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.35">
@@ -488,7 +488,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="2">
-        <v>60000</v>
+        <v>0</v>
       </c>
       <c r="D3" s="2">
         <v>5000</v>
@@ -500,7 +500,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="2">
-        <v>0</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -511,7 +511,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="2">
-        <v>60000</v>
+        <v>0</v>
       </c>
       <c r="D4" s="2">
         <v>5000</v>
@@ -523,7 +523,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="2">
-        <v>0</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -534,7 +534,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="2">
-        <v>60000</v>
+        <v>0</v>
       </c>
       <c r="D5" s="2">
         <v>5000</v>
@@ -546,7 +546,7 @@
         <v>0</v>
       </c>
       <c r="G5" s="2">
-        <v>0</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.35">
@@ -557,7 +557,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="2">
-        <v>60000</v>
+        <v>0</v>
       </c>
       <c r="D6" s="2">
         <v>5000</v>
@@ -569,7 +569,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="2">
-        <v>0</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -580,7 +580,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="2">
-        <v>60000</v>
+        <v>0</v>
       </c>
       <c r="D7" s="2">
         <v>5000</v>
@@ -592,7 +592,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="2">
-        <v>0</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -603,7 +603,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="2">
-        <v>60000</v>
+        <v>0</v>
       </c>
       <c r="D8" s="2">
         <v>5000</v>
@@ -615,7 +615,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="2">
-        <v>0</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -626,7 +626,7 @@
         <v>14</v>
       </c>
       <c r="C9" s="2">
-        <v>60000</v>
+        <v>0</v>
       </c>
       <c r="D9" s="2">
         <v>5000</v>
@@ -638,7 +638,7 @@
         <v>0</v>
       </c>
       <c r="G9" s="2">
-        <v>0</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -649,7 +649,7 @@
         <v>15</v>
       </c>
       <c r="C10" s="2">
-        <v>60000</v>
+        <v>0</v>
       </c>
       <c r="D10" s="2">
         <v>5000</v>
@@ -661,7 +661,7 @@
         <v>0</v>
       </c>
       <c r="G10" s="2">
-        <v>0</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -672,7 +672,7 @@
         <v>16</v>
       </c>
       <c r="C11" s="2">
-        <v>60000</v>
+        <v>0</v>
       </c>
       <c r="D11" s="2">
         <v>5000</v>
@@ -684,7 +684,7 @@
         <v>0</v>
       </c>
       <c r="G11" s="2">
-        <v>0</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -695,7 +695,7 @@
         <v>17</v>
       </c>
       <c r="C12" s="2">
-        <v>60000</v>
+        <v>0</v>
       </c>
       <c r="D12" s="2">
         <v>5000</v>
@@ -707,7 +707,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="2">
-        <v>0</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -718,7 +718,7 @@
         <v>18</v>
       </c>
       <c r="C13" s="2">
-        <v>60000</v>
+        <v>0</v>
       </c>
       <c r="D13" s="2">
         <v>5000</v>
@@ -730,7 +730,7 @@
         <v>0</v>
       </c>
       <c r="G13" s="2">
-        <v>0</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -741,7 +741,7 @@
         <v>9</v>
       </c>
       <c r="C14" s="2">
-        <v>60000</v>
+        <v>0</v>
       </c>
       <c r="D14" s="2">
         <v>5000</v>
@@ -753,7 +753,7 @@
         <v>0</v>
       </c>
       <c r="G14" s="2">
-        <v>0</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -764,7 +764,7 @@
         <v>10</v>
       </c>
       <c r="C15" s="2">
-        <v>60000</v>
+        <v>0</v>
       </c>
       <c r="D15" s="2">
         <v>5000</v>
@@ -776,7 +776,7 @@
         <v>0</v>
       </c>
       <c r="G15" s="2">
-        <v>0</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -787,7 +787,7 @@
         <v>11</v>
       </c>
       <c r="C16" s="2">
-        <v>60000</v>
+        <v>0</v>
       </c>
       <c r="D16" s="2">
         <v>5000</v>
@@ -799,7 +799,7 @@
         <v>0</v>
       </c>
       <c r="G16" s="2">
-        <v>0</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
@@ -810,7 +810,7 @@
         <v>12</v>
       </c>
       <c r="C17" s="2">
-        <v>60000</v>
+        <v>0</v>
       </c>
       <c r="D17" s="2">
         <v>5000</v>
@@ -822,7 +822,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="2">
-        <v>0</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
@@ -833,7 +833,7 @@
         <v>13</v>
       </c>
       <c r="C18" s="2">
-        <v>60000</v>
+        <v>0</v>
       </c>
       <c r="D18" s="2">
         <v>5000</v>
@@ -845,7 +845,7 @@
         <v>0</v>
       </c>
       <c r="G18" s="2">
-        <v>0</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
@@ -856,7 +856,7 @@
         <v>7</v>
       </c>
       <c r="C19" s="2">
-        <v>60000</v>
+        <v>0</v>
       </c>
       <c r="D19" s="2">
         <v>5000</v>
@@ -868,7 +868,7 @@
         <v>0</v>
       </c>
       <c r="G19" s="2">
-        <v>0</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
@@ -879,7 +879,7 @@
         <v>8</v>
       </c>
       <c r="C20" s="2">
-        <v>60000</v>
+        <v>0</v>
       </c>
       <c r="D20" s="2">
         <v>5000</v>
@@ -891,7 +891,7 @@
         <v>0</v>
       </c>
       <c r="G20" s="2">
-        <v>0</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
@@ -914,7 +914,7 @@
         <v>1032291</v>
       </c>
       <c r="G21" s="2">
-        <v>0</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
@@ -928,7 +928,7 @@
         <v>1075000</v>
       </c>
       <c r="D22" s="2">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="E22" s="2">
         <v>450000</v>
@@ -937,7 +937,7 @@
         <v>1032291</v>
       </c>
       <c r="G22" s="2">
-        <v>0</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
@@ -951,7 +951,7 @@
         <v>1075000</v>
       </c>
       <c r="D23" s="2">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="E23" s="2">
         <v>450000</v>
@@ -960,7 +960,7 @@
         <v>1032291</v>
       </c>
       <c r="G23" s="2">
-        <v>0</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
@@ -974,7 +974,7 @@
         <v>1075000</v>
       </c>
       <c r="D24" s="2">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="E24" s="2">
         <v>450000</v>
@@ -983,7 +983,7 @@
         <v>1032291</v>
       </c>
       <c r="G24" s="2">
-        <v>0</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
@@ -997,7 +997,7 @@
         <v>1075000</v>
       </c>
       <c r="D25" s="2">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="E25" s="2">
         <v>450000</v>
@@ -1006,7 +1006,7 @@
         <v>238541</v>
       </c>
       <c r="G25" s="2">
-        <v>0</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
@@ -1020,7 +1020,7 @@
         <v>1225000</v>
       </c>
       <c r="D26" s="2">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="E26" s="2">
         <v>450000</v>
@@ -1029,7 +1029,7 @@
         <v>246874</v>
       </c>
       <c r="G26" s="2">
-        <v>0</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
@@ -1043,7 +1043,7 @@
         <v>650000</v>
       </c>
       <c r="D27" s="2">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="E27" s="2">
         <v>450000</v>
@@ -1052,7 +1052,7 @@
         <v>246874</v>
       </c>
       <c r="G27" s="2">
-        <v>0</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
@@ -1066,7 +1066,7 @@
         <v>850000</v>
       </c>
       <c r="D28" s="2">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="E28" s="2">
         <v>450000</v>
@@ -1075,7 +1075,7 @@
         <v>246874</v>
       </c>
       <c r="G28" s="2">
-        <v>0</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
@@ -1089,7 +1089,7 @@
         <v>850000</v>
       </c>
       <c r="D29" s="2">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="E29" s="2">
         <v>450000</v>
@@ -1098,7 +1098,7 @@
         <v>246874</v>
       </c>
       <c r="G29" s="2">
-        <v>0</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
@@ -1112,7 +1112,7 @@
         <v>850000</v>
       </c>
       <c r="D30" s="2">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="E30" s="2">
         <v>450000</v>
@@ -1121,7 +1121,7 @@
         <v>246874</v>
       </c>
       <c r="G30" s="2">
-        <v>0</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
@@ -1135,7 +1135,7 @@
         <v>1155000</v>
       </c>
       <c r="D31" s="2">
-        <v>5000</v>
+        <v>15000</v>
       </c>
       <c r="E31" s="2">
         <v>450000</v>
@@ -1144,7 +1144,7 @@
         <v>246874</v>
       </c>
       <c r="G31" s="2">
-        <v>0</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
@@ -1158,7 +1158,7 @@
         <v>870000</v>
       </c>
       <c r="D32" s="2">
-        <v>5000</v>
+        <v>15000</v>
       </c>
       <c r="E32" s="2">
         <v>450000</v>
@@ -1167,7 +1167,7 @@
         <v>246874</v>
       </c>
       <c r="G32" s="2">
-        <v>0</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
@@ -1181,7 +1181,7 @@
         <v>870000</v>
       </c>
       <c r="D33" s="2">
-        <v>5000</v>
+        <v>15000</v>
       </c>
       <c r="E33" s="2">
         <v>450000</v>
@@ -1190,7 +1190,7 @@
         <v>246874</v>
       </c>
       <c r="G33" s="2">
-        <v>0</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
@@ -1204,7 +1204,7 @@
         <v>870000</v>
       </c>
       <c r="D34" s="2">
-        <v>5000</v>
+        <v>15000</v>
       </c>
       <c r="E34" s="2">
         <v>450000</v>
@@ -1213,7 +1213,467 @@
         <v>246874</v>
       </c>
       <c r="G34" s="2">
-        <v>0</v>
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35" s="2">
+        <v>2025</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" s="2">
+        <v>870000</v>
+      </c>
+      <c r="D35" s="2">
+        <v>15000</v>
+      </c>
+      <c r="E35" s="2">
+        <v>450000</v>
+      </c>
+      <c r="F35" s="2">
+        <v>246874</v>
+      </c>
+      <c r="G35" s="2">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" s="2">
+        <v>2025</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" s="2">
+        <v>870000</v>
+      </c>
+      <c r="D36" s="2">
+        <v>15000</v>
+      </c>
+      <c r="E36" s="2">
+        <v>450000</v>
+      </c>
+      <c r="F36" s="2">
+        <v>246874</v>
+      </c>
+      <c r="G36" s="2">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" s="2">
+        <v>2025</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" s="2">
+        <v>870000</v>
+      </c>
+      <c r="D37" s="2">
+        <v>15000</v>
+      </c>
+      <c r="E37" s="2">
+        <v>450000</v>
+      </c>
+      <c r="F37" s="2">
+        <v>246874</v>
+      </c>
+      <c r="G37" s="2">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38" s="2">
+        <v>2025</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="2">
+        <v>870000</v>
+      </c>
+      <c r="D38" s="2">
+        <v>15000</v>
+      </c>
+      <c r="E38" s="2">
+        <v>450000</v>
+      </c>
+      <c r="F38" s="2">
+        <v>246874</v>
+      </c>
+      <c r="G38" s="2">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" s="2">
+        <v>2025</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" s="2">
+        <v>870000</v>
+      </c>
+      <c r="D39" s="2">
+        <v>15000</v>
+      </c>
+      <c r="E39" s="2">
+        <v>450000</v>
+      </c>
+      <c r="F39" s="2">
+        <v>246874</v>
+      </c>
+      <c r="G39" s="2">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40" s="2">
+        <v>2025</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="2">
+        <v>870000</v>
+      </c>
+      <c r="D40" s="2">
+        <v>15000</v>
+      </c>
+      <c r="E40" s="2">
+        <v>450000</v>
+      </c>
+      <c r="F40" s="2">
+        <v>246874</v>
+      </c>
+      <c r="G40" s="2">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41" s="2">
+        <v>2025</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" s="2">
+        <v>870000</v>
+      </c>
+      <c r="D41" s="2">
+        <v>15000</v>
+      </c>
+      <c r="E41" s="2">
+        <v>450000</v>
+      </c>
+      <c r="F41" s="2">
+        <v>246874</v>
+      </c>
+      <c r="G41" s="2">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42" s="2">
+        <v>2025</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42" s="2">
+        <v>870000</v>
+      </c>
+      <c r="D42" s="2">
+        <v>15000</v>
+      </c>
+      <c r="E42" s="2">
+        <v>450000</v>
+      </c>
+      <c r="F42" s="2">
+        <v>246874</v>
+      </c>
+      <c r="G42" s="2">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A43" s="2">
+        <v>2026</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" s="2">
+        <v>870000</v>
+      </c>
+      <c r="D43" s="2">
+        <v>15000</v>
+      </c>
+      <c r="E43" s="2">
+        <v>450000</v>
+      </c>
+      <c r="F43" s="2">
+        <v>246874</v>
+      </c>
+      <c r="G43" s="2">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A44" s="2">
+        <v>2026</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" s="2">
+        <v>870000</v>
+      </c>
+      <c r="D44" s="2">
+        <v>15000</v>
+      </c>
+      <c r="E44" s="2">
+        <v>450000</v>
+      </c>
+      <c r="F44" s="2">
+        <v>246874</v>
+      </c>
+      <c r="G44" s="2">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A45" s="2">
+        <v>2026</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45" s="2">
+        <v>870000</v>
+      </c>
+      <c r="D45" s="2">
+        <v>15000</v>
+      </c>
+      <c r="E45" s="2">
+        <v>450000</v>
+      </c>
+      <c r="F45" s="2">
+        <v>246874</v>
+      </c>
+      <c r="G45" s="2">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A46" s="2">
+        <v>2026</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C46" s="2">
+        <v>870000</v>
+      </c>
+      <c r="D46" s="2">
+        <v>15000</v>
+      </c>
+      <c r="E46" s="2">
+        <v>450000</v>
+      </c>
+      <c r="F46" s="2">
+        <v>246874</v>
+      </c>
+      <c r="G46" s="2">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A47" s="2">
+        <v>2026</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C47" s="2">
+        <v>870000</v>
+      </c>
+      <c r="D47" s="2">
+        <v>15000</v>
+      </c>
+      <c r="E47" s="2">
+        <v>450000</v>
+      </c>
+      <c r="F47" s="2">
+        <v>246874</v>
+      </c>
+      <c r="G47" s="2">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A48" s="2">
+        <v>2026</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C48" s="2">
+        <v>870000</v>
+      </c>
+      <c r="D48" s="2">
+        <v>15000</v>
+      </c>
+      <c r="E48" s="2">
+        <v>450000</v>
+      </c>
+      <c r="F48" s="2">
+        <v>246874</v>
+      </c>
+      <c r="G48" s="2">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A49" s="2">
+        <v>2026</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C49" s="2">
+        <v>870000</v>
+      </c>
+      <c r="D49" s="2">
+        <v>15000</v>
+      </c>
+      <c r="E49" s="2">
+        <v>450000</v>
+      </c>
+      <c r="F49" s="2">
+        <v>246874</v>
+      </c>
+      <c r="G49" s="2">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A50" s="2">
+        <v>2026</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50" s="2">
+        <v>870000</v>
+      </c>
+      <c r="D50" s="2">
+        <v>15000</v>
+      </c>
+      <c r="E50" s="2">
+        <v>450000</v>
+      </c>
+      <c r="F50" s="2">
+        <v>246874</v>
+      </c>
+      <c r="G50" s="2">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A51" s="2">
+        <v>2026</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C51" s="2">
+        <v>870000</v>
+      </c>
+      <c r="D51" s="2">
+        <v>15000</v>
+      </c>
+      <c r="E51" s="2">
+        <v>450000</v>
+      </c>
+      <c r="F51" s="2">
+        <v>246874</v>
+      </c>
+      <c r="G51" s="2">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A52" s="2">
+        <v>2026</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52" s="2">
+        <v>870000</v>
+      </c>
+      <c r="D52" s="2">
+        <v>15000</v>
+      </c>
+      <c r="E52" s="2">
+        <v>450000</v>
+      </c>
+      <c r="F52" s="2">
+        <v>246874</v>
+      </c>
+      <c r="G52" s="2">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A53" s="2">
+        <v>2026</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C53" s="2">
+        <v>870000</v>
+      </c>
+      <c r="D53" s="2">
+        <v>15000</v>
+      </c>
+      <c r="E53" s="2">
+        <v>450000</v>
+      </c>
+      <c r="F53" s="2">
+        <v>246874</v>
+      </c>
+      <c r="G53" s="2">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A54" s="2">
+        <v>2026</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C54" s="2">
+        <v>870000</v>
+      </c>
+      <c r="D54" s="2">
+        <v>15000</v>
+      </c>
+      <c r="E54" s="2">
+        <v>450000</v>
+      </c>
+      <c r="F54" s="2">
+        <v>246874</v>
+      </c>
+      <c r="G54" s="2">
+        <v>30000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mise à jour charge.xls
</commit_message>
<xml_diff>
--- a/charges.xlsx
+++ b/charges.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fatou Sène Dieng\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fatou Sène Dieng\mon_projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E01E8B-E146-4949-9FDF-141FEA36AA39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F2DEF3-6365-4764-A2A3-A15D248E5D22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>